<commit_message>
Add Playwright test cases for Singlish to Sinhala translator
</commit_message>
<xml_diff>
--- a/IT23722286_TestCases.xlsx
+++ b/IT23722286_TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akind\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akind\Desktop\IT23722286\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C558189-7164-431C-9F98-7A6AC35DFC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A62FC1F-067E-4478-8D7C-4FA0420E0312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="11380" windowHeight="13370" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Test cases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="134">
   <si>
     <t>TC ID</t>
   </si>
@@ -316,155 +316,49 @@
     </r>
   </si>
   <si>
-    <t>Pos_UI_0001</t>
-  </si>
-  <si>
-    <t>Sinhala output updates automatically in real-time</t>
-  </si>
-  <si>
-    <t>man gedhara yanavaa</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sinhala output should update automatically while typing and display: </t>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t>මන් ගෙදර යනවා</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sinhala output is updated automatically while typing and display: </t>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Output updates correctly as the user types the full sentence.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
     </r>
     <r>
       <rPr>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="Iskoola Pota"/>
-        <family val="2"/>
-      </rPr>
-      <t>මන් ගෙදර යනවා</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Output updates correctly as the user types the full sentence.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>No UI lag or freezing observed for short input.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Usability flow (real-time conversion)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
       <t>Simple sentence</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>·</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Real-time output update behavior</t>
     </r>
   </si>
   <si>
@@ -1113,6 +1007,332 @@
       </rPr>
       <t>  Real-time output update behavior</t>
     </r>
+  </si>
+  <si>
+    <t>Pos_Fun_05</t>
+  </si>
+  <si>
+    <t>Informal greeting question</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Informal greeting is translated correctly with preserved tone.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>  Greeting / request / response</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>  Interrogative</t>
+    </r>
+  </si>
+  <si>
+    <t>Neg_Fun_05</t>
+  </si>
+  <si>
+    <t>Informal time-related request</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Slang and informal timing words reduce translation accuracy..</t>
+    </r>
+  </si>
+  <si>
+    <t>Pos_Fun_06</t>
+  </si>
+  <si>
+    <t>Paragraph style daily scenario</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Long input is converted with correct structure and preserved meaning.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>  Slang</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>  Formatting (paragraph)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Complex sentence</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Robustness validation</t>
+    </r>
+  </si>
+  <si>
+    <t>Pos_Fun_07</t>
+  </si>
+  <si>
+    <t>Proper noun handling</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>   Accuracy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> validation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>   Simple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> sentence</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>  Name/Places</t>
+    </r>
+  </si>
+  <si>
+    <t>lQQkaa maathaa</t>
+  </si>
+  <si>
+    <t>ලංකා මාතා</t>
+  </si>
+  <si>
+    <t>adha udha mama office yanna laesthi vunee, habaeyi vahina hindha paare loku traffic ekak. bus eka ganna kalin mama phone eka aran message baluvaa. ethakota thamaa dhakkee loku kunatuvak aevilla kiyala</t>
+  </si>
+  <si>
+    <t>අද උද මම office යන්න ලැස්ති වුනේ, හබැයි වහින හින්ද පාරෙ ලොකු traffic එකක්. bus එක ගන්න කලින් මම phone එක අරන් message බලුවා. එතකොට තමා දක්කේ ලොකු කුනටුවක් ඇවිල්ල කියල</t>
+  </si>
+  <si>
+    <t>malli zoom meeting eka ganna  daen</t>
+  </si>
+  <si>
+    <t>මල්ලි zoom meeting එක ගන්න ඩැන්</t>
+  </si>
+  <si>
+    <t>yaluvane kohoma dha</t>
+  </si>
+  <si>
+    <t>යලුවනෙ කොහොම ද</t>
+  </si>
+  <si>
+    <t>Pos_Fun_08</t>
+  </si>
+  <si>
+    <t>Mixed social media sentence</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>English brand name is preserved while Sinhala structure remains accurate.</t>
+    </r>
+  </si>
+  <si>
+    <t>TikTok balanavaa ne oyalaa addict venava</t>
+  </si>
+  <si>
+    <t>TikTok බලනවා නේ ඔයලා addict වෙනව</t>
+  </si>
+  <si>
+    <t>මල්ලි zoom meeting එක ගන්න දැන්ම</t>
+  </si>
+  <si>
+    <t>awith balanna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">අwඉත් බලන්න
+</t>
+  </si>
+  <si>
+    <t>ඇවිත් බලන්න</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1256,22 +1476,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1290,6 +1498,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1571,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="50" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1621,42 +1844,42 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="4"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
@@ -1665,13 +1888,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="4"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="2" t="s">
         <v>12</v>
       </c>
@@ -1680,127 +1903,127 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="4"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="A6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>58</v>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="4"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="4"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="4"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="A10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="4"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1809,512 +2032,774 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="4"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="A13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="D13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="4"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="16" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="4"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="A17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="5"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="4"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="4"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>58</v>
+      <c r="D21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="5"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="4"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="4"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="4"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>58</v>
+      <c r="D25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="4"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="5"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="5"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="4"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="5"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="5"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="4"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="5"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B33" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H29" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="5"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="5"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="34" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="5"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="4"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="5"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="4"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="5"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="4"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="5"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="4"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="14"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="14"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="15"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="2" t="s">
-        <v>32</v>
+      <c r="I53" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="10"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="10"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="11"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="70">
+  <mergeCells count="98">
     <mergeCell ref="B25:B28"/>
     <mergeCell ref="D33:D36"/>
     <mergeCell ref="E33:E36"/>
@@ -2373,6 +2858,18 @@
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="F2:F5"/>
     <mergeCell ref="G10:G12"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="D53:D56"/>
+    <mergeCell ref="E53:E56"/>
+    <mergeCell ref="F53:F56"/>
+    <mergeCell ref="G53:G56"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="B37:B40"/>
     <mergeCell ref="C37:C40"/>
@@ -2380,11 +2877,27 @@
     <mergeCell ref="E37:E40"/>
     <mergeCell ref="F37:F40"/>
     <mergeCell ref="G37:G40"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="G41:G44"/>
+    <mergeCell ref="F41:F44"/>
+    <mergeCell ref="E41:E44"/>
+    <mergeCell ref="D41:D44"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="F45:F48"/>
+    <mergeCell ref="G45:G48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="C49:C52"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="F49:F52"/>
+    <mergeCell ref="G49:G52"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="C45:C48"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="E45:E48"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>